<commit_message>
Implemented own keepAlive packets
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC65475-21DD-4AE0-895B-F780BAF0F2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8609EA10-DFA0-4F7E-A0C7-DC563BBC2A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="152">
   <si>
     <t>Packet</t>
   </si>
@@ -481,9 +481,6 @@
   </si>
   <si>
     <t>entity teleport vs entity position?</t>
-  </si>
-  <si>
-    <t>see pull request on node-minecraft-protocol</t>
   </si>
 </sst>
 </file>
@@ -525,11 +522,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -543,14 +561,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -569,9 +580,61 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -853,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,7 +925,7 @@
     <col min="3" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.26953125" customWidth="1"/>
+    <col min="6" max="6" width="81.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
@@ -928,7 +991,7 @@
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>95</v>
@@ -939,29 +1002,29 @@
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
         <v>95</v>
@@ -972,29 +1035,29 @@
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
@@ -1005,7 +1068,7 @@
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -1016,7 +1079,7 @@
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
         <v>95</v>
@@ -1027,43 +1090,43 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
         <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="F20" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
         <v>95</v>
@@ -1074,7 +1137,7 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -1085,7 +1148,7 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
@@ -1096,7 +1159,7 @@
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>95</v>
@@ -1107,7 +1170,7 @@
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
         <v>95</v>
@@ -1118,18 +1181,18 @@
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
         <v>95</v>
@@ -1140,18 +1203,18 @@
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
         <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
         <v>95</v>
@@ -1162,65 +1225,62 @@
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
         <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
         <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
         <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
         <v>95</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
         <v>95</v>
@@ -1229,98 +1289,101 @@
         <v>141</v>
       </c>
       <c r="F35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
         <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="F36" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
         <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="F38" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
         <v>95</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
         <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="F42" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
         <v>95</v>
@@ -1331,7 +1394,7 @@
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
         <v>95</v>
@@ -1342,32 +1405,32 @@
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
         <v>95</v>
       </c>
       <c r="E45" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
         <v>95</v>
       </c>
       <c r="E46" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="F46" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
         <v>95</v>
@@ -1378,7 +1441,7 @@
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
         <v>95</v>
@@ -1389,7 +1452,7 @@
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
         <v>95</v>
@@ -1400,7 +1463,7 @@
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
         <v>95</v>
@@ -1411,7 +1474,7 @@
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
         <v>95</v>
@@ -1422,7 +1485,7 @@
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
         <v>95</v>
@@ -1433,7 +1496,7 @@
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
         <v>95</v>
@@ -1444,7 +1507,7 @@
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
         <v>95</v>
@@ -1455,13 +1518,13 @@
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
         <v>95</v>
       </c>
       <c r="E55" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.35">
@@ -1918,7 +1981,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>96</v>
       </c>
@@ -1929,7 +1992,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>97</v>
       </c>
@@ -1940,7 +2003,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>98</v>
       </c>
@@ -1951,7 +2014,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>99</v>
       </c>
@@ -1962,7 +2025,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>100</v>
       </c>
@@ -1973,7 +2036,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>101</v>
       </c>
@@ -1984,7 +2047,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>102</v>
       </c>
@@ -1995,7 +2058,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>18</v>
       </c>
@@ -2006,7 +2069,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>20</v>
       </c>
@@ -2017,7 +2080,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>103</v>
       </c>
@@ -2028,7 +2091,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>104</v>
       </c>
@@ -2039,7 +2102,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>26</v>
       </c>
@@ -2050,7 +2113,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>105</v>
       </c>
@@ -2061,7 +2124,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>106</v>
       </c>
@@ -2072,7 +2135,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>107</v>
       </c>
@@ -2083,7 +2146,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
         <v>34</v>
       </c>
@@ -2091,10 +2154,7 @@
         <v>136</v>
       </c>
       <c r="E112" t="s">
-        <v>141</v>
-      </c>
-      <c r="F112" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.35">
@@ -2440,28 +2500,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D143">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>"Server"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Client"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"Server"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38 F35:F36 F20 F40 F42 F46 F5 F91 F112 E5:E143">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"Fully implemented"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"Partly implemented"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+      <formula>"Tried"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>"Not started"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E143 F37 F34:F35 F19 F39 F41 F45 F5 F91 F112">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"N/A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"Not started"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Tried"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Partly implemented"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Fully implemented"</formula>
+  <conditionalFormatting sqref="E5:E143">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented CustomError for some functions and events
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31738730-146D-4DFE-97D9-65E14CCE5F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE03FCA-A392-4262-8F69-BF9E555CE91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="154">
   <si>
     <t>Packet</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>entity teleport vs entity position?</t>
+  </si>
+  <si>
+    <t>status == 5</t>
+  </si>
+  <si>
+    <t>obj.mouse == 0: return ??, use destructuring</t>
   </si>
 </sst>
 </file>
@@ -522,63 +528,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color theme="0"/>
@@ -916,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,7 +875,7 @@
     <col min="3" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
@@ -1981,7 +1931,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>96</v>
       </c>
@@ -1992,7 +1942,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>97</v>
       </c>
@@ -2003,7 +1953,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>98</v>
       </c>
@@ -2014,7 +1964,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>99</v>
       </c>
@@ -2025,7 +1975,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>100</v>
       </c>
@@ -2036,7 +1986,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>101</v>
       </c>
@@ -2047,7 +1997,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>102</v>
       </c>
@@ -2058,7 +2008,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>18</v>
       </c>
@@ -2069,7 +2019,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>20</v>
       </c>
@@ -2080,7 +2030,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>103</v>
       </c>
@@ -2091,7 +2041,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>104</v>
       </c>
@@ -2102,7 +2052,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>26</v>
       </c>
@@ -2113,7 +2063,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>105</v>
       </c>
@@ -2124,7 +2074,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>106</v>
       </c>
@@ -2132,10 +2082,13 @@
         <v>136</v>
       </c>
       <c r="E110" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="F110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>107</v>
       </c>
@@ -2146,7 +2099,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
         <v>34</v>
       </c>
@@ -2157,7 +2110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
         <v>108</v>
       </c>
@@ -2168,7 +2121,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
         <v>109</v>
       </c>
@@ -2179,7 +2132,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
         <v>110</v>
       </c>
@@ -2190,7 +2143,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
         <v>111</v>
       </c>
@@ -2201,7 +2154,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
         <v>112</v>
       </c>
@@ -2212,7 +2165,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
         <v>46</v>
       </c>
@@ -2223,7 +2176,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
         <v>113</v>
       </c>
@@ -2234,7 +2187,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
         <v>114</v>
       </c>
@@ -2245,7 +2198,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
         <v>115</v>
       </c>
@@ -2256,7 +2209,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
         <v>51</v>
       </c>
@@ -2267,7 +2220,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
         <v>116</v>
       </c>
@@ -2275,10 +2228,13 @@
         <v>136</v>
       </c>
       <c r="E123" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="F123" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
         <v>117</v>
       </c>
@@ -2289,7 +2245,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
         <v>118</v>
       </c>
@@ -2300,7 +2256,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
         <v>119</v>
       </c>
@@ -2311,7 +2267,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C127" t="s">
         <v>120</v>
       </c>
@@ -2322,7 +2278,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
         <v>121</v>
       </c>
@@ -2500,32 +2456,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D143">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Server"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Client"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38 F35:F36 F20 F40 F42 F46 F5 F91 F112 E5:E143">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+  <conditionalFormatting sqref="F38 F35:F36 F20 F40 F42 F46 F5 F91 F112 E5:E143 F123 F110">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E143">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="E5:E143 F123 F110">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Made maxPlayers and motd defaultable
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE03FCA-A392-4262-8F69-BF9E555CE91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D877F4-51DE-4071-B433-967210ADE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented pattern recognition for CustomError
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D877F4-51DE-4071-B433-967210ADE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2B9D1D-B0EA-49A0-9300-820FC7C0421A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -867,7 +867,7 @@
   <dimension ref="C4:F143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+      <selection activeCell="XFD1048576" sqref="XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added fancy stats to packets spreadsheet
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7990FA76-390C-42F3-845E-83DCD56CF83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203D5D30-BB8A-45E0-9C58-AABFB1AEA350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Packets" sheetId="1" r:id="rId1"/>
+    <sheet name="Stats" sheetId="2" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="157">
   <si>
     <t>Packet</t>
   </si>
@@ -108,9 +118,6 @@
     <t>plugin message</t>
   </si>
   <si>
-    <t>named sounds effect</t>
-  </si>
-  <si>
     <t>disconnect</t>
   </si>
   <si>
@@ -487,6 +494,18 @@
   </si>
   <si>
     <t>obj.mouse == 0: return ??, use destructuring</t>
+  </si>
+  <si>
+    <t>named sound effect</t>
+  </si>
+  <si>
+    <t>Packet coverage</t>
+  </si>
+  <si>
+    <t>Status weights</t>
+  </si>
+  <si>
+    <t>working</t>
   </si>
 </sst>
 </file>
@@ -502,12 +521,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -522,13 +547,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -866,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.35">
@@ -897,13 +941,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.35">
@@ -911,10 +955,10 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.35">
@@ -922,10 +966,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.35">
@@ -933,21 +977,21 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
@@ -955,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
@@ -966,10 +1010,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.35">
@@ -977,10 +1021,10 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.35">
@@ -988,10 +1032,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
@@ -999,10 +1043,10 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.35">
@@ -1010,10 +1054,10 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.35">
@@ -1021,10 +1065,10 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.35">
@@ -1032,10 +1076,10 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.35">
@@ -1043,10 +1087,10 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.35">
@@ -1054,10 +1098,10 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.35">
@@ -1065,13 +1109,13 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.35">
@@ -1079,10 +1123,10 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.35">
@@ -1090,10 +1134,10 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.35">
@@ -1101,10 +1145,10 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.35">
@@ -1112,10 +1156,10 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.35">
@@ -1123,10 +1167,10 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.35">
@@ -1134,10 +1178,10 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.35">
@@ -1145,10 +1189,10 @@
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.35">
@@ -1156,10 +1200,10 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.35">
@@ -1167,10 +1211,10 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.35">
@@ -1178,10 +1222,10 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.35">
@@ -1189,7 +1233,7 @@
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
         <v>139</v>
@@ -1200,10 +1244,10 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.35">
@@ -1211,7 +1255,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
         <v>139</v>
@@ -1222,10 +1266,13 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
         <v>140</v>
+      </c>
+      <c r="F34" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.35">
@@ -1233,10 +1280,10 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F35" t="s">
         <v>143</v>
@@ -1247,13 +1294,10 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.35">
@@ -1261,10 +1305,13 @@
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="F37" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.35">
@@ -1272,13 +1319,10 @@
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.35">
@@ -1286,10 +1330,13 @@
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
         <v>140</v>
+      </c>
+      <c r="F39" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.35">
@@ -1297,13 +1344,10 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.35">
@@ -1311,10 +1355,13 @@
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E41" t="s">
         <v>140</v>
+      </c>
+      <c r="F41" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.35">
@@ -1322,13 +1369,10 @@
         <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
-      </c>
-      <c r="F42" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.35">
@@ -1336,10 +1380,10 @@
         <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.35">
@@ -1347,10 +1391,10 @@
         <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.35">
@@ -1358,10 +1402,13 @@
         <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" t="s">
         <v>140</v>
+      </c>
+      <c r="F45" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.35">
@@ -1369,13 +1416,10 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E46" t="s">
         <v>139</v>
-      </c>
-      <c r="F46" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.35">
@@ -1383,10 +1427,10 @@
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.35">
@@ -1394,10 +1438,10 @@
         <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.35">
@@ -1405,10 +1449,10 @@
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.35">
@@ -1416,10 +1460,10 @@
         <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.35">
@@ -1427,10 +1471,10 @@
         <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.35">
@@ -1438,10 +1482,10 @@
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.35">
@@ -1449,10 +1493,10 @@
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.35">
@@ -1460,21 +1504,21 @@
         <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C55" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.35">
@@ -1482,10 +1526,10 @@
         <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.35">
@@ -1493,7 +1537,7 @@
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E57" t="s">
         <v>139</v>
@@ -1504,10 +1548,10 @@
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.35">
@@ -1515,10 +1559,10 @@
         <v>57</v>
       </c>
       <c r="D59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.35">
@@ -1526,10 +1570,10 @@
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.35">
@@ -1537,10 +1581,10 @@
         <v>59</v>
       </c>
       <c r="D61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.35">
@@ -1548,10 +1592,10 @@
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.35">
@@ -1559,10 +1603,10 @@
         <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.35">
@@ -1570,10 +1614,10 @@
         <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.35">
@@ -1581,10 +1625,10 @@
         <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.35">
@@ -1592,10 +1636,10 @@
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.35">
@@ -1603,10 +1647,10 @@
         <v>65</v>
       </c>
       <c r="D67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.35">
@@ -1614,10 +1658,10 @@
         <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.35">
@@ -1625,7 +1669,7 @@
         <v>67</v>
       </c>
       <c r="D69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E69" t="s">
         <v>139</v>
@@ -1636,10 +1680,10 @@
         <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.35">
@@ -1647,10 +1691,10 @@
         <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.35">
@@ -1658,10 +1702,10 @@
         <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.35">
@@ -1669,10 +1713,10 @@
         <v>71</v>
       </c>
       <c r="D73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.35">
@@ -1680,10 +1724,10 @@
         <v>72</v>
       </c>
       <c r="D74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.35">
@@ -1691,10 +1735,10 @@
         <v>73</v>
       </c>
       <c r="D75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.35">
@@ -1702,10 +1746,10 @@
         <v>74</v>
       </c>
       <c r="D76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="3:5" x14ac:dyDescent="0.35">
@@ -1713,10 +1757,10 @@
         <v>75</v>
       </c>
       <c r="D77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.35">
@@ -1724,7 +1768,7 @@
         <v>76</v>
       </c>
       <c r="D78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E78" t="s">
         <v>139</v>
@@ -1735,10 +1779,10 @@
         <v>77</v>
       </c>
       <c r="D79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E79" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.35">
@@ -1746,10 +1790,10 @@
         <v>78</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.35">
@@ -1757,10 +1801,10 @@
         <v>79</v>
       </c>
       <c r="D81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.35">
@@ -1768,10 +1812,10 @@
         <v>80</v>
       </c>
       <c r="D82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.35">
@@ -1779,10 +1823,10 @@
         <v>81</v>
       </c>
       <c r="D83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.35">
@@ -1790,7 +1834,7 @@
         <v>82</v>
       </c>
       <c r="D84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E84" t="s">
         <v>139</v>
@@ -1801,211 +1845,211 @@
         <v>83</v>
       </c>
       <c r="D85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E87" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E88" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E90" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E96" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E99" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D100" t="s">
+        <v>135</v>
+      </c>
+      <c r="E100" t="s">
         <v>136</v>
-      </c>
-      <c r="E100" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E103" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.35">
@@ -2013,10 +2057,10 @@
         <v>18</v>
       </c>
       <c r="D104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E104" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.35">
@@ -2024,32 +2068,32 @@
         <v>20</v>
       </c>
       <c r="D105" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E105" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D106" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E107" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.35">
@@ -2057,435 +2101,545 @@
         <v>26</v>
       </c>
       <c r="D108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E108" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D109" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E109" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E110" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F110" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D111" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E111" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E112" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D113" t="s">
+        <v>135</v>
+      </c>
+      <c r="E113" t="s">
         <v>136</v>
-      </c>
-      <c r="E113" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="114" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E114" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E115" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D116" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E116" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D117" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E117" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D118" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E120" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="121" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E121" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E122" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E123" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F123" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E124" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D125" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E125" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E126" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C127" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D127" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E127" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E128" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C129" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E129" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C130" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D130" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E130" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C131" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D131" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C132" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D132" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E132" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="133" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C133" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D133" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E133" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D134" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E134" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="135" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C135" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E135" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="136" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C136" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E136" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="137" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C137" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C138" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C139" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D139" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="140" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C140" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D140" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D141" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C142" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D142" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C143" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D143" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E143" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D143">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Server"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Client"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38 F35:F36 F20 F40 F42 F46 F5 F91 F112 E5:E143 F123 F110">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="F37 F34:F35 F20 F39 F41 F45 F5 F91 F112 F123 F110 E5:E143">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E143 F123 F110">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F123 F110 E5:E143">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F031A1-1BAA-40E9-B49C-760E1954E8E5}">
+  <dimension ref="C4:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="1">
+        <f>((COUNTIF(Packets!E5:E143, "fully implemented") * Settings!D5) + (COUNTIF(Packets!E5:E143, "working implemented") * Settings!D6) + (COUNTIF(Packets!E5:E143, "partly implemented") * Settings!D7) + (COUNTIF(Packets!E5:E143, "tried") * Settings!D8) + (COUNTIF(Packets!E5:E143, "not started") * Settings!D9))/ROWS(Packets!E5:E143)*100</f>
+        <v>22.374100719424458</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:D34">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA79DE60-9FBD-4AFE-B354-2911D8201B1C}">
+  <dimension ref="C4:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented set position flags
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C28A78-D748-4C2D-9612-0A528D7048B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE201A6A-09EA-403F-9A78-05703F72B57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="157">
   <si>
     <t>Packet</t>
   </si>
@@ -506,9 +506,6 @@
   </si>
   <si>
     <t>see player info and Spawn player</t>
-  </si>
-  <si>
-    <t>implement flags, every flag defines if that thing is relative or absolute</t>
   </si>
 </sst>
 </file>
@@ -936,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -945,7 +942,7 @@
     <col min="3" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
@@ -1602,11 +1599,9 @@
         <v>94</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>157</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C57" s="6" t="s">
@@ -2699,7 +2694,7 @@
   <dimension ref="C4:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2715,7 +2710,7 @@
       </c>
       <c r="D4" s="2">
         <f>((COUNTIF(Packets!E5:E143, "fully implemented") * Settings!D5) + (COUNTIF(Packets!E5:E143, "working implemented") * Settings!D6) + (COUNTIF(Packets!E5:E143, "partly implemented") * Settings!D7) + (COUNTIF(Packets!E5:E143, "tried") * Settings!D8) + (COUNTIF(Packets!E5:E143, "not started") * Settings!D9))/ROWS(Packets!E5:E143)*100</f>
-        <v>26.546762589928065</v>
+        <v>26.762589928057558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved serverList defaults into separate object
</commit_message>
<xml_diff>
--- a/packets.xlsx
+++ b/packets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Desktop\Programmeren\minecraft-server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DA3432-9922-46DB-8AD1-034027AD35D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3E0AD7-64AC-49CD-8F86-DF6D5408AC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,9 +469,6 @@
     <t>see file</t>
   </si>
   <si>
-    <t>worlds, viewDistance</t>
-  </si>
-  <si>
     <t>check which if to send rotation and/or position</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>q</t>
+  </si>
+  <si>
+    <t>worlds, viewDistance, maxPlayers</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.35">
@@ -973,7 +973,7 @@
         <v>140</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.35">
@@ -1023,7 +1023,7 @@
         <v>137</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
@@ -1037,7 +1037,7 @@
         <v>137</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
@@ -1156,10 +1156,10 @@
         <v>94</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>139</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.35">
@@ -1421,7 +1421,7 @@
         <v>140</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.35">
@@ -1471,7 +1471,7 @@
         <v>140</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.35">
@@ -1497,7 +1497,7 @@
         <v>139</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.35">
@@ -1958,7 +1958,7 @@
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C86" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>94</v>
@@ -2027,7 +2027,7 @@
         <v>140</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.35">
@@ -2413,7 +2413,7 @@
         <v>140</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="3:6" x14ac:dyDescent="0.35">
@@ -2711,7 +2711,7 @@
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" s="2">
         <f>((COUNTIF(Packets!E5:E143, "fully implemented") * Settings!D5) + (COUNTIF(Packets!E5:E143, "working implemented") * Settings!D6) + (COUNTIF(Packets!E5:E143, "partly implemented") * Settings!D7) + (COUNTIF(Packets!E5:E143, "tried") * Settings!D8) + (COUNTIF(Packets!E5:E143, "not started") * Settings!D9))/ROWS(Packets!E5:E143)*100</f>
@@ -2756,7 +2756,7 @@
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.35">
@@ -2769,7 +2769,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6">
         <v>0.8</v>

</xml_diff>